<commit_message>
Bugfix, add step buttons
Fixed bugs with two schemes
Add step buttons to setup slider
Hero ids are a single format now
Separated some of the formatting code to a separate script.
</commit_message>
<xml_diff>
--- a/data/schemes.xlsx
+++ b/data/schemes.xlsx
@@ -1178,8 +1178,8 @@
   <dimension ref="A1:Y124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W62" sqref="W62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1392,9 +1392,6 @@
       <c r="R6" t="s">
         <v>36</v>
       </c>
-      <c r="S6" t="s">
-        <v>167</v>
-      </c>
       <c r="V6" t="s">
         <v>154</v>
       </c>
@@ -2272,6 +2269,9 @@
       </c>
       <c r="R50" t="s">
         <v>137</v>
+      </c>
+      <c r="V50" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:23">

</xml_diff>

<commit_message>
fix card text spacing
</commit_message>
<xml_diff>
--- a/data/schemes.xlsx
+++ b/data/schemes.xlsx
@@ -1658,10 +1658,10 @@
   <dimension ref="A1:AG132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2576,32 +2576,32 @@
         <v>363</v>
       </c>
     </row>
-    <row r="31" spans="1:31" s="6" customFormat="1">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:31" s="4" customFormat="1">
+      <c r="A31" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="4">
         <v>2</v>
       </c>
-      <c r="P31" s="6" t="s">
+      <c r="P31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="U31" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC31" s="6" t="s">
+      <c r="U31" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="AD31" s="6" t="s">
+      <c r="AD31" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="AE31" s="6" t="s">
+      <c r="AE31" s="4" t="s">
         <v>426</v>
       </c>
     </row>
@@ -4040,26 +4040,26 @@
         <v>352</v>
       </c>
     </row>
-    <row r="85" spans="1:33" s="6" customFormat="1">
-      <c r="A85" s="6" t="s">
+    <row r="85" spans="1:33" s="4" customFormat="1">
+      <c r="A85" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C85" s="4">
         <v>11</v>
       </c>
-      <c r="N85" s="6">
+      <c r="N85" s="4">
         <v>2</v>
       </c>
-      <c r="P85" s="6" t="s">
+      <c r="P85" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AD85" s="6" t="s">
+      <c r="AD85" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="AE85" s="6" t="s">
+      <c r="AE85" s="4" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added script to get img
Script added to download images
</commit_message>
<xml_diff>
--- a/data/schemes.xlsx
+++ b/data/schemes.xlsx
@@ -572,9 +572,6 @@
     <t>Deadpool Kills the Marvel Universe</t>
   </si>
   <si>
-    <t>Deadpool Wants a Chimichanga</t>
-  </si>
-  <si>
     <t>Deadpool Writes a Scheme</t>
   </si>
   <si>
@@ -1302,6 +1299,9 @@
   </si>
   <si>
     <t>Put player tokens into the sewers</t>
+  </si>
+  <si>
+    <t>Deadpool Wants A Chimichanga</t>
   </si>
 </sst>
 </file>
@@ -1658,10 +1658,10 @@
   <dimension ref="A1:AG132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1765,31 +1765,31 @@
         <v>101</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="AF1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -1812,13 +1812,13 @@
         <v>117</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AD2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AE2" t="s">
         <v>332</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:33">
@@ -1850,24 +1850,24 @@
         <v>98</v>
       </c>
       <c r="Y3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Z3">
         <v>30</v>
       </c>
       <c r="AD3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C4">
         <v>11</v>
@@ -1876,16 +1876,16 @@
         <v>45</v>
       </c>
       <c r="Q4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S4">
         <v>1</v>
       </c>
       <c r="AD4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AE4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -1908,10 +1908,10 @@
         <v>34</v>
       </c>
       <c r="AD5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -1931,10 +1931,10 @@
         <v>140</v>
       </c>
       <c r="AD6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AE6" t="s">
         <v>383</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:33">
@@ -1957,10 +1957,10 @@
         <v>36</v>
       </c>
       <c r="AD7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:33">
@@ -1980,10 +1980,10 @@
         <v>42</v>
       </c>
       <c r="AD8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:33">
@@ -2009,13 +2009,13 @@
         <v>44</v>
       </c>
       <c r="AC9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AD9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AE9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:33">
@@ -2038,10 +2038,10 @@
         <v>161</v>
       </c>
       <c r="AD10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:33">
@@ -2061,13 +2061,13 @@
         <v>51</v>
       </c>
       <c r="AC11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AD11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -2087,13 +2087,13 @@
         <v>40</v>
       </c>
       <c r="Z12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AD12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -2113,13 +2113,13 @@
         <v>151</v>
       </c>
       <c r="AC13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AD13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -2139,13 +2139,13 @@
         <v>39</v>
       </c>
       <c r="AC14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AD14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:33">
@@ -2168,10 +2168,10 @@
         <v>1</v>
       </c>
       <c r="AD15" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE15" t="s">
         <v>346</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -2191,16 +2191,16 @@
         <v>40</v>
       </c>
       <c r="Z16" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC16" t="s">
         <v>271</v>
       </c>
-      <c r="AC16" t="s">
-        <v>272</v>
-      </c>
       <c r="AD16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -2226,13 +2226,13 @@
         <v>55</v>
       </c>
       <c r="AC17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AD17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -2252,10 +2252,10 @@
         <v>145</v>
       </c>
       <c r="AD18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AE18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:31">
@@ -2278,13 +2278,13 @@
         <v>153</v>
       </c>
       <c r="AC19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AD19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -2307,10 +2307,10 @@
         <v>78</v>
       </c>
       <c r="AD20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:31">
@@ -2330,10 +2330,10 @@
         <v>56</v>
       </c>
       <c r="AD21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:31">
@@ -2362,13 +2362,13 @@
         <v>113</v>
       </c>
       <c r="AC22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AD22" t="s">
+        <v>412</v>
+      </c>
+      <c r="AE22" t="s">
         <v>413</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -2385,10 +2385,10 @@
         <v>41</v>
       </c>
       <c r="AD23" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -2408,10 +2408,10 @@
         <v>44</v>
       </c>
       <c r="AD24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -2434,10 +2434,10 @@
         <v>1</v>
       </c>
       <c r="AD25" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE25" t="s">
         <v>402</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="26" spans="1:31" s="4" customFormat="1">
@@ -2448,7 +2448,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L26" s="4">
         <v>1</v>
@@ -2466,15 +2466,15 @@
         <v>96</v>
       </c>
       <c r="AD26" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AE26" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:31" s="4" customFormat="1">
       <c r="A27" s="4" t="s">
-        <v>185</v>
+        <v>428</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>59</v>
@@ -2492,21 +2492,21 @@
         <v>61</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y27" s="4">
         <v>12</v>
       </c>
       <c r="AD27" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AE27" s="4" t="s">
         <v>367</v>
-      </c>
-      <c r="AE27" s="4" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
@@ -2521,18 +2521,18 @@
         <v>96</v>
       </c>
       <c r="AD28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AE28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="4" customFormat="1">
       <c r="A29" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C29" s="4">
         <v>9</v>
@@ -2541,18 +2541,18 @@
         <v>42</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AD29" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AE29" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
@@ -2570,21 +2570,21 @@
         <v>160</v>
       </c>
       <c r="AD30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="31" spans="1:31" s="4" customFormat="1">
       <c r="A31" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>424</v>
       </c>
       <c r="N31" s="4">
         <v>2</v>
@@ -2596,13 +2596,13 @@
         <v>1</v>
       </c>
       <c r="AC31" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="AD31" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="AE31" s="4" t="s">
         <v>425</v>
-      </c>
-      <c r="AD31" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="AE31" s="4" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:31" s="4" customFormat="1">
@@ -2622,18 +2622,18 @@
         <v>119</v>
       </c>
       <c r="AC32" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AD32" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AE32" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:33">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33" t="s">
         <v>93</v>
@@ -2666,15 +2666,15 @@
         <v>161</v>
       </c>
       <c r="AD33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE33" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:33">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -2692,13 +2692,13 @@
         <v>1</v>
       </c>
       <c r="AD34" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AE34">
         <v>1</v>
       </c>
       <c r="AF34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AG34">
         <v>1</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="35" spans="1:33">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -2724,21 +2724,21 @@
         <v>63</v>
       </c>
       <c r="AD35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:33">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L36">
         <v>1</v>
@@ -2747,15 +2747,15 @@
         <v>42</v>
       </c>
       <c r="AD36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:33">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B37" t="s">
         <v>59</v>
@@ -2773,10 +2773,10 @@
         <v>66</v>
       </c>
       <c r="AD37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AE37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="38" spans="1:33">
@@ -2799,13 +2799,13 @@
         <v>61</v>
       </c>
       <c r="AC38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AD38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AE38" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="1:33" s="4" customFormat="1">
@@ -2828,16 +2828,16 @@
         <v>112</v>
       </c>
       <c r="V39" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z39" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD39" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE39" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40" spans="1:33" s="4" customFormat="1">
@@ -2854,13 +2854,13 @@
         <v>41</v>
       </c>
       <c r="AC40" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AD40" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AE40" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="41" spans="1:33">
@@ -2886,15 +2886,15 @@
         <v>61</v>
       </c>
       <c r="AD41" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AE41" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="42" spans="1:33">
       <c r="A42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B42" t="s">
         <v>67</v>
@@ -2909,18 +2909,18 @@
         <v>68</v>
       </c>
       <c r="AA42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD42" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AE42" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="43" spans="1:33">
       <c r="A43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B43" t="s">
         <v>67</v>
@@ -2938,18 +2938,18 @@
         <v>2</v>
       </c>
       <c r="AC43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AD43" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AE43" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:33">
       <c r="A44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
@@ -2967,15 +2967,15 @@
         <v>69</v>
       </c>
       <c r="AD44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE44" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" spans="1:33">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
@@ -2993,47 +2993,47 @@
         <v>71</v>
       </c>
       <c r="AD45" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AE45" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="46" spans="1:33" s="6" customFormat="1">
-      <c r="A46" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B46" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" s="4" customFormat="1">
+      <c r="A46" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="N46" s="6">
+      <c r="C46" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="N46" s="4">
         <v>2</v>
       </c>
-      <c r="P46" s="6" t="s">
+      <c r="P46" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="R46" s="6" t="s">
+      <c r="R46" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="T46" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC46" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="AD46" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE46" s="6" t="s">
-        <v>348</v>
+      <c r="T46" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC46" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AD46" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="AE46" s="4" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="47" spans="1:33">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B47" t="s">
         <v>107</v>
@@ -3051,15 +3051,15 @@
         <v>110</v>
       </c>
       <c r="AD47" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:33">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B48" t="s">
         <v>43</v>
@@ -3074,10 +3074,10 @@
         <v>162</v>
       </c>
       <c r="AD48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AE48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="49" spans="1:33">
@@ -3097,13 +3097,13 @@
         <v>159</v>
       </c>
       <c r="AC49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AD49" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE49" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="50" spans="1:33">
@@ -3120,15 +3120,15 @@
         <v>41</v>
       </c>
       <c r="AD50" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AE50" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:33">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B51" t="s">
         <v>67</v>
@@ -3146,18 +3146,18 @@
         <v>72</v>
       </c>
       <c r="AC51" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AD51" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AE51" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" spans="1:33">
       <c r="A52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
@@ -3169,10 +3169,10 @@
         <v>41</v>
       </c>
       <c r="AD52" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:33">
@@ -3201,16 +3201,16 @@
         <v>134</v>
       </c>
       <c r="AC53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AD53" t="s">
+        <v>384</v>
+      </c>
+      <c r="AE53">
+        <v>1</v>
+      </c>
+      <c r="AF53" t="s">
         <v>385</v>
-      </c>
-      <c r="AE53">
-        <v>1</v>
-      </c>
-      <c r="AF53" t="s">
-        <v>386</v>
       </c>
       <c r="AG53">
         <v>1</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="54" spans="1:33">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B54" t="s">
         <v>137</v>
@@ -3236,15 +3236,15 @@
         <v>1</v>
       </c>
       <c r="AD54" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AE54" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:33">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B55" t="s">
         <v>93</v>
@@ -3265,18 +3265,18 @@
         <v>1</v>
       </c>
       <c r="Y55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD55" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE55" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:33">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
         <v>35</v>
@@ -3297,15 +3297,15 @@
         <v>61</v>
       </c>
       <c r="AD56" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="57" spans="1:33">
       <c r="A57" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B57" t="s">
         <v>150</v>
@@ -3326,18 +3326,18 @@
         <v>61</v>
       </c>
       <c r="AC57" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AD57" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE57" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="58" spans="1:33">
       <c r="A58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B58" t="s">
         <v>70</v>
@@ -3352,18 +3352,18 @@
         <v>42</v>
       </c>
       <c r="AC58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AD58" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AE58" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="59" spans="1:33" s="4" customFormat="1">
       <c r="A59" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>73</v>
@@ -3381,13 +3381,13 @@
         <v>1</v>
       </c>
       <c r="AC59" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AD59" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE59" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="60" spans="1:33">
@@ -3410,15 +3410,15 @@
         <v>1</v>
       </c>
       <c r="AD60" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AE60" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61" spans="1:33">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" t="s">
         <v>37</v>
@@ -3430,10 +3430,10 @@
         <v>41</v>
       </c>
       <c r="AD61" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE61" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="62" spans="1:33">
@@ -3453,15 +3453,15 @@
         <v>42</v>
       </c>
       <c r="AD62" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AE62" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:33">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
         <v>53</v>
@@ -3479,10 +3479,10 @@
         <v>42</v>
       </c>
       <c r="AD63" t="s">
+        <v>358</v>
+      </c>
+      <c r="AE63" t="s">
         <v>359</v>
-      </c>
-      <c r="AE63" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="64" spans="1:33">
@@ -3502,16 +3502,16 @@
         <v>45</v>
       </c>
       <c r="Q64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AD64" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:31" s="4" customFormat="1">
@@ -3537,18 +3537,18 @@
         <v>76</v>
       </c>
       <c r="AC65" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AD65" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE65" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="1:31">
       <c r="A66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B66" t="s">
         <v>58</v>
@@ -3563,15 +3563,15 @@
         <v>39</v>
       </c>
       <c r="AD66" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE66" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="67" spans="1:31">
       <c r="A67" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B67" t="s">
         <v>39</v>
@@ -3595,18 +3595,18 @@
         <v>123</v>
       </c>
       <c r="Z67" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD67" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AE67" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="68" spans="1:31">
       <c r="A68" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B68" t="s">
         <v>2</v>
@@ -3630,15 +3630,15 @@
         <v>12</v>
       </c>
       <c r="AD68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE68" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="69" spans="1:31">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
         <v>31</v>
@@ -3662,15 +3662,15 @@
         <v>99</v>
       </c>
       <c r="AD69" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE69" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="70" spans="1:31" s="4" customFormat="1">
       <c r="A70" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>107</v>
@@ -3685,18 +3685,18 @@
         <v>109</v>
       </c>
       <c r="AC70" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AD70" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE70" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="71" spans="1:31">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B71" t="s">
         <v>2</v>
@@ -3714,15 +3714,15 @@
         <v>1</v>
       </c>
       <c r="AD71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE71" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72" spans="1:31">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
         <v>35</v>
@@ -3743,15 +3743,15 @@
         <v>61</v>
       </c>
       <c r="AD72" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73" spans="1:31">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B73" t="s">
         <v>31</v>
@@ -3763,15 +3763,15 @@
         <v>41</v>
       </c>
       <c r="AD73" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE73" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74" spans="1:31">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B74" t="s">
         <v>53</v>
@@ -3792,15 +3792,15 @@
         <v>77</v>
       </c>
       <c r="AD74" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE74" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:31">
       <c r="A75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B75" t="s">
         <v>49</v>
@@ -3821,10 +3821,10 @@
         <v>30</v>
       </c>
       <c r="AD75" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="76" spans="1:31">
@@ -3844,15 +3844,15 @@
         <v>41</v>
       </c>
       <c r="AD76" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AE76" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" spans="1:31">
       <c r="A77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -3864,15 +3864,15 @@
         <v>41</v>
       </c>
       <c r="AD77" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE77" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:31">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B78" t="s">
         <v>35</v>
@@ -3890,15 +3890,15 @@
         <v>1</v>
       </c>
       <c r="AD78" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE78" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:31">
       <c r="A79" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B79" t="s">
         <v>116</v>
@@ -3913,15 +3913,15 @@
         <v>39</v>
       </c>
       <c r="AD79" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AE79" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="80" spans="1:31">
       <c r="A80" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B80" t="s">
         <v>37</v>
@@ -3933,10 +3933,10 @@
         <v>41</v>
       </c>
       <c r="AD80" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="81" spans="1:33">
@@ -3956,15 +3956,15 @@
         <v>50</v>
       </c>
       <c r="AD81" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AE81" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="1:33">
       <c r="A82" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B82" t="s">
         <v>2</v>
@@ -3985,18 +3985,18 @@
         <v>18</v>
       </c>
       <c r="AC82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AD82" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE82" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:33">
       <c r="A83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B83" t="s">
         <v>150</v>
@@ -4011,15 +4011,15 @@
         <v>39</v>
       </c>
       <c r="AD83" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AE83" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="84" spans="1:33">
       <c r="A84" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B84" t="s">
         <v>35</v>
@@ -4034,18 +4034,18 @@
         <v>161</v>
       </c>
       <c r="AD84" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AE84" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="85" spans="1:33" s="4" customFormat="1">
       <c r="A85" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C85" s="4">
         <v>11</v>
@@ -4057,15 +4057,15 @@
         <v>50</v>
       </c>
       <c r="AD85" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AE85" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="86" spans="1:33">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B86" t="s">
         <v>53</v>
@@ -4089,10 +4089,10 @@
         <v>61</v>
       </c>
       <c r="AD86" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE86" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="87" spans="1:33">
@@ -4115,18 +4115,18 @@
         <v>1</v>
       </c>
       <c r="AC87" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AD87" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AE87" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="1:33">
       <c r="A88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B88" t="s">
         <v>137</v>
@@ -4141,24 +4141,24 @@
         <v>41</v>
       </c>
       <c r="AC88" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AD88" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AE88" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="89" spans="1:33">
       <c r="A89" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P89" t="s">
         <v>50</v>
@@ -4167,16 +4167,16 @@
         <v>135</v>
       </c>
       <c r="AC89" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AD89" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE89">
+        <v>1</v>
+      </c>
+      <c r="AF89" t="s">
         <v>387</v>
-      </c>
-      <c r="AE89">
-        <v>1</v>
-      </c>
-      <c r="AF89" t="s">
-        <v>388</v>
       </c>
       <c r="AG89">
         <v>1</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="90" spans="1:33">
       <c r="A90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B90" t="s">
         <v>2</v>
@@ -4211,13 +4211,13 @@
         <v>102</v>
       </c>
       <c r="AC90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AD90" t="s">
+        <v>336</v>
+      </c>
+      <c r="AE90" t="s">
         <v>337</v>
-      </c>
-      <c r="AE90" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="91" spans="1:33">
@@ -4237,15 +4237,15 @@
         <v>81</v>
       </c>
       <c r="AD91" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE91" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="1:33" s="4" customFormat="1">
       <c r="A92" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>137</v>
@@ -4260,15 +4260,15 @@
         <v>47</v>
       </c>
       <c r="AD92" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AE92" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="93" spans="1:33">
       <c r="A93" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B93" t="s">
         <v>107</v>
@@ -4283,18 +4283,18 @@
         <v>109</v>
       </c>
       <c r="AC93" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AD93" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE93" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="94" spans="1:33">
       <c r="A94" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
         <v>67</v>
@@ -4312,15 +4312,15 @@
         <v>61</v>
       </c>
       <c r="AD94" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AE94" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="95" spans="1:33">
       <c r="A95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B95" t="s">
         <v>58</v>
@@ -4338,18 +4338,18 @@
         <v>82</v>
       </c>
       <c r="AC95" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AD95" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE95" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="96" spans="1:33" s="6" customFormat="1">
       <c r="A96" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>49</v>
@@ -4367,18 +4367,18 @@
         <v>1</v>
       </c>
       <c r="AC96" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AD96" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AE96" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="97" spans="1:33">
       <c r="A97" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B97" t="s">
         <v>73</v>
@@ -4399,15 +4399,15 @@
         <v>83</v>
       </c>
       <c r="AD97" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE97" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="98" spans="1:33">
       <c r="A98" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B98" t="s">
         <v>93</v>
@@ -4422,15 +4422,15 @@
         <v>42</v>
       </c>
       <c r="AD98" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AE98" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="99" spans="1:33">
       <c r="A99" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B99" t="s">
         <v>53</v>
@@ -4445,15 +4445,15 @@
         <v>1</v>
       </c>
       <c r="AD99" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE99" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:33">
       <c r="A100" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B100" t="s">
         <v>107</v>
@@ -4465,21 +4465,21 @@
         <v>41</v>
       </c>
       <c r="AD100" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE100" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" spans="1:33">
       <c r="A101" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L101">
         <v>2</v>
@@ -4491,10 +4491,10 @@
         <v>155</v>
       </c>
       <c r="AD101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE101" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="102" spans="1:33" s="6" customFormat="1">
@@ -4517,13 +4517,13 @@
         <v>1</v>
       </c>
       <c r="AC102" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AD102" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AE102" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="103" spans="1:33" s="4" customFormat="1">
@@ -4546,18 +4546,18 @@
         <v>1</v>
       </c>
       <c r="AC103" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AD103" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AE103" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="104" spans="1:33">
       <c r="A104" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B104" t="s">
         <v>31</v>
@@ -4572,18 +4572,18 @@
         <v>40</v>
       </c>
       <c r="Z104" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD104" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE104" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="105" spans="1:33">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B105" t="s">
         <v>73</v>
@@ -4598,18 +4598,18 @@
         <v>39</v>
       </c>
       <c r="AD105" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AE105" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="106" spans="1:33" s="4" customFormat="1">
       <c r="A106" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C106" s="4">
         <v>11</v>
@@ -4621,15 +4621,15 @@
         <v>1</v>
       </c>
       <c r="AD106" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AE106" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="107" spans="1:33">
       <c r="A107" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B107" t="s">
         <v>31</v>
@@ -4650,13 +4650,13 @@
         <v>103</v>
       </c>
       <c r="AC107" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AD107" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE107" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="108" spans="1:33">
@@ -4673,10 +4673,10 @@
         <v>41</v>
       </c>
       <c r="AD108" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AE108" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="109" spans="1:33" s="4" customFormat="1">
@@ -4699,18 +4699,18 @@
         <v>147</v>
       </c>
       <c r="AC109" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AD109" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AE109" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="110" spans="1:33">
       <c r="A110" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B110" t="s">
         <v>58</v>
@@ -4728,15 +4728,15 @@
         <v>85</v>
       </c>
       <c r="AD110" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE110" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="111" spans="1:33">
       <c r="A111" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B111" t="s">
         <v>58</v>
@@ -4751,10 +4751,10 @@
         <v>41</v>
       </c>
       <c r="AD111" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE111" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="112" spans="1:33">
@@ -4783,13 +4783,13 @@
         <v>131</v>
       </c>
       <c r="AD112" t="s">
+        <v>388</v>
+      </c>
+      <c r="AE112">
+        <v>1</v>
+      </c>
+      <c r="AF112" t="s">
         <v>389</v>
-      </c>
-      <c r="AE112">
-        <v>1</v>
-      </c>
-      <c r="AF112" t="s">
-        <v>390</v>
       </c>
       <c r="AG112">
         <v>1</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="113" spans="1:31" s="4" customFormat="1">
       <c r="A113" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>70</v>
@@ -4812,18 +4812,18 @@
         <v>86</v>
       </c>
       <c r="X113" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD113" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AE113" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="114" spans="1:31">
       <c r="A114" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B114" t="s">
         <v>2</v>
@@ -4841,18 +4841,18 @@
         <v>40</v>
       </c>
       <c r="Z114" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD114" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE114" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="115" spans="1:31">
       <c r="A115" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B115" t="s">
         <v>58</v>
@@ -4873,13 +4873,13 @@
         <v>100</v>
       </c>
       <c r="AC115" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AD115" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AE115" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="116" spans="1:31">
@@ -4896,18 +4896,18 @@
         <v>41</v>
       </c>
       <c r="AA116" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD116" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AE116" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="117" spans="1:31">
       <c r="A117" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B117" t="s">
         <v>43</v>
@@ -4919,41 +4919,41 @@
         <v>41</v>
       </c>
       <c r="AA117" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AD117" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AE117" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="118" spans="1:31" s="6" customFormat="1">
-      <c r="A118" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" s="4" customFormat="1">
+      <c r="A118" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C118" s="4">
+        <v>10</v>
+      </c>
+      <c r="P118" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC118" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B118" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="C118" s="6">
-        <v>10</v>
-      </c>
-      <c r="P118" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC118" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="AD118" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="AE118" s="6" t="s">
+      <c r="AD118" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="AE118" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="119" spans="1:31" s="4" customFormat="1">
       <c r="A119" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>53</v>
@@ -4971,27 +4971,27 @@
         <v>84</v>
       </c>
       <c r="Y119" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AC119" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AD119" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE119" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="120" spans="1:31">
       <c r="A120" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B120" t="s">
         <v>116</v>
       </c>
       <c r="C120" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P120" t="s">
         <v>50</v>
@@ -5000,15 +5000,15 @@
         <v>128</v>
       </c>
       <c r="AD120" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AE120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:31">
       <c r="A121" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
         <v>116</v>
@@ -5023,41 +5023,41 @@
         <v>39</v>
       </c>
       <c r="AC121" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD121" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AE121" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="122" spans="1:31">
       <c r="A122" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B122" t="s">
         <v>144</v>
       </c>
       <c r="C122" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P122" t="s">
         <v>41</v>
       </c>
       <c r="AD122" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AE122" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="123" spans="1:31" s="4" customFormat="1">
       <c r="A123" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C123" s="4">
         <v>14</v>
@@ -5066,21 +5066,21 @@
         <v>50</v>
       </c>
       <c r="AD123" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AE123" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="124" spans="1:31">
       <c r="A124" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B124" t="s">
         <v>70</v>
       </c>
       <c r="C124" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P124" t="s">
         <v>50</v>
@@ -5089,15 +5089,15 @@
         <v>89</v>
       </c>
       <c r="AD124" t="s">
+        <v>377</v>
+      </c>
+      <c r="AE124" t="s">
         <v>378</v>
-      </c>
-      <c r="AE124" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:31">
       <c r="A125" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B125" t="s">
         <v>35</v>
@@ -5112,15 +5112,15 @@
         <v>88</v>
       </c>
       <c r="AD125" t="s">
+        <v>349</v>
+      </c>
+      <c r="AE125" t="s">
         <v>350</v>
-      </c>
-      <c r="AE125" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="126" spans="1:31">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B126" t="s">
         <v>2</v>
@@ -5132,18 +5132,18 @@
         <v>41</v>
       </c>
       <c r="AD126" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE126" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="127" spans="1:31">
       <c r="A127" t="s">
+        <v>415</v>
+      </c>
+      <c r="B127" t="s">
         <v>416</v>
-      </c>
-      <c r="B127" t="s">
-        <v>417</v>
       </c>
       <c r="C127">
         <v>11</v>
@@ -5152,18 +5152,18 @@
         <v>50</v>
       </c>
       <c r="R127" t="s">
+        <v>417</v>
+      </c>
+      <c r="AD127" t="s">
         <v>418</v>
       </c>
-      <c r="AD127" t="s">
+      <c r="AE127" t="s">
         <v>419</v>
-      </c>
-      <c r="AE127" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="128" spans="1:31">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B128" t="s">
         <v>139</v>
@@ -5181,15 +5181,15 @@
         <v>141</v>
       </c>
       <c r="AD128" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AE128" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="129" spans="1:31">
       <c r="A129" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B129" t="s">
         <v>73</v>
@@ -5201,10 +5201,10 @@
         <v>41</v>
       </c>
       <c r="AD129" t="s">
+        <v>393</v>
+      </c>
+      <c r="AE129" t="s">
         <v>394</v>
-      </c>
-      <c r="AE129" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="130" spans="1:31" s="4" customFormat="1">
@@ -5224,18 +5224,18 @@
         <v>108</v>
       </c>
       <c r="AC130" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AD130" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AE130" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="131" spans="1:31">
       <c r="A131" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B131" t="s">
         <v>53</v>
@@ -5253,21 +5253,21 @@
         <v>90</v>
       </c>
       <c r="Y131" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AC131" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD131" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AE131" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="132" spans="1:31">
       <c r="A132" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B132" t="s">
         <v>31</v>
@@ -5279,10 +5279,10 @@
         <v>41</v>
       </c>
       <c r="AD132" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AE132" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -5501,26 +5501,26 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B26" t="s">
         <v>263</v>
-      </c>
-      <c r="B26" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data bug anti mutant hatred
wound count was listed for wrong scheme
</commit_message>
<xml_diff>
--- a/data/schemes.xlsx
+++ b/data/schemes.xlsx
@@ -1676,10 +1676,10 @@
   <dimension ref="A1:AG136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE101" sqref="AE101"/>
+      <selection pane="bottomRight" activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1870,9 +1870,6 @@
       <c r="Y3" t="s">
         <v>315</v>
       </c>
-      <c r="Z3">
-        <v>30</v>
-      </c>
       <c r="AD3" t="s">
         <v>406</v>
       </c>
@@ -1924,6 +1921,9 @@
       </c>
       <c r="R5" t="s">
         <v>34</v>
+      </c>
+      <c r="Z5">
+        <v>30</v>
       </c>
       <c r="AD5" t="s">
         <v>406</v>

</xml_diff>